<commit_message>
Removed negative signs from production and degradation rates
</commit_message>
<xml_diff>
--- a/data/GRNmap_input_workbooks/14-genes_35-edges_BK-dGLN3-fam_Sigmoid_estimation.xlsx
+++ b/data/GRNmap_input_workbooks/14-genes_35-edges_BK-dGLN3-fam_Sigmoid_estimation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" tabRatio="905" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="905"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="7" r:id="rId1"/>
@@ -240,7 +240,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="190">
+  <cellStyleXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -389,6 +389,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -459,7 +463,7 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="147" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="147" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="190">
+  <cellStyles count="194">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -554,6 +558,8 @@
     <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -648,6 +654,8 @@
     <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="147"/>
   </cellStyles>
@@ -980,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1004,7 +1012,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>-0.2009</v>
+        <v>0.2009</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1012,7 +1020,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>-0.30809999999999998</v>
+        <v>0.30809999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1020,7 +1028,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>-0.1925</v>
+        <v>0.1925</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1028,7 +1036,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>-0.32240000000000002</v>
+        <v>0.32240000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1036,7 +1044,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>-0.27179999999999999</v>
+        <v>0.27179999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1044,7 +1052,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="9">
-        <v>-9.9000000000000005E-2</v>
+        <v>9.9000000000000005E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1052,7 +1060,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>-0.40770000000000001</v>
+        <v>0.40770000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1060,7 +1068,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>-0.27729999999999999</v>
+        <v>0.27729999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1068,7 +1076,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>-0.69310000000000005</v>
+        <v>0.69310000000000005</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1076,7 +1084,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>-0.28289999999999998</v>
+        <v>0.28289999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1084,7 +1092,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>-0.32240000000000002</v>
+        <v>0.32240000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1092,7 +1100,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>-0.55449999999999999</v>
+        <v>0.55449999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1100,7 +1108,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>-0.17330000000000001</v>
+        <v>0.17330000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1108,7 +1116,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>-0.72960000000000003</v>
+        <v>0.72960000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -1468,7 +1476,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1491,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>-0.10050000000000001</v>
+        <v>0.10050000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1499,7 +1507,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="9">
-        <v>-0.154</v>
+        <v>0.154</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1507,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>-9.6299999999999997E-2</v>
+        <v>9.6299999999999997E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1515,7 +1523,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>-0.16120000000000001</v>
+        <v>0.16120000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1523,7 +1531,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>-0.13589999999999999</v>
+        <v>0.13589999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1531,7 +1539,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>-4.9500000000000002E-2</v>
+        <v>4.9500000000000002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1539,7 +1547,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>-0.2039</v>
+        <v>0.2039</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1547,7 +1555,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>-0.1386</v>
+        <v>0.1386</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1555,7 +1563,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>-0.34660000000000002</v>
+        <v>0.34660000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1563,7 +1571,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>-0.14149999999999999</v>
+        <v>0.14149999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1571,7 +1579,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>-0.16120000000000001</v>
+        <v>0.16120000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1579,7 +1587,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>-0.27729999999999999</v>
+        <v>0.27729999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1587,7 +1595,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>-8.6599999999999996E-2</v>
+        <v>8.6599999999999996E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1595,7 +1603,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>-0.36480000000000001</v>
+        <v>0.36480000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -4857,7 +4865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>